<commit_message>
commit avant la veille tech
</commit_message>
<xml_diff>
--- a/doc/8-BTS_SIO-Annexe8-1-Tableau_de_synthe_se-Epreuve-E4-BTS_SIO_2024 XIONG Teddy.xlsx
+++ b/doc/8-BTS_SIO-Annexe8-1-Tableau_de_synthe_se-Epreuve-E4-BTS_SIO_2024 XIONG Teddy.xlsx
@@ -8,22 +8,22 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Utilisateur\Documents\portfolio\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3AD1725-0B44-4B5E-8D6C-733582505CB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77FB5A24-9A43-488F-A551-D5DC894122D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3690" yWindow="3270" windowWidth="18000" windowHeight="9270" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tableau de synthèse Épreuve E4" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'Tableau de synthèse Épreuve E4'!$A$1:$H$33</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Tableau de synthèse Épreuve E4'!$A$1:$H$32</definedName>
   </definedNames>
   <calcPr calcId="101716"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
   <si>
     <t>Gérer le patrimoine informatique</t>
   </si>
@@ -126,10 +126,6 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">AP2 bis - Réalisation site web static ( HTML, CSS)
-</t>
-  </si>
-  <si>
     <t>AP2 - Réalisation site web dynamique (HTML, CSS, PHP, SQL)</t>
   </si>
   <si>
@@ -139,9 +135,6 @@
     <t>AP3 - Réalisation application web + Framework web</t>
   </si>
   <si>
-    <t>AP4 - Réalisation application lours (java) + .jar</t>
-  </si>
-  <si>
     <t>Création d'une interface logiciel client lourd - outil mesure atmosphère</t>
   </si>
   <si>
@@ -155,6 +148,9 @@
   </si>
   <si>
     <t>N° candidat : 02212505167</t>
+  </si>
+  <si>
+    <t>AP4 - Réalisation application lourd (java) + .jar</t>
   </si>
 </sst>
 </file>
@@ -779,13 +775,13 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="27" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="27" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1099,8 +1095,8 @@
   </sheetPr>
   <dimension ref="A1:AQ83"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="U6" sqref="U6"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1147,7 +1143,7 @@
       <c r="D3" s="28"/>
       <c r="E3" s="29"/>
       <c r="F3" s="33" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="G3" s="28"/>
       <c r="H3" s="34"/>
@@ -1174,16 +1170,16 @@
       </c>
     </row>
     <row r="5" spans="1:43" ht="39.950000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="47" t="s">
-        <v>35</v>
-      </c>
-      <c r="B5" s="45"/>
-      <c r="C5" s="45"/>
-      <c r="D5" s="45"/>
-      <c r="E5" s="45"/>
-      <c r="F5" s="45"/>
-      <c r="G5" s="45"/>
-      <c r="H5" s="46"/>
+      <c r="A5" s="45" t="s">
+        <v>33</v>
+      </c>
+      <c r="B5" s="46"/>
+      <c r="C5" s="46"/>
+      <c r="D5" s="46"/>
+      <c r="E5" s="46"/>
+      <c r="F5" s="46"/>
+      <c r="G5" s="46"/>
+      <c r="H5" s="47"/>
     </row>
     <row r="6" spans="1:43" ht="90" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="35" t="s">
@@ -1369,10 +1365,10 @@
       <c r="B10" s="10"/>
       <c r="C10" s="17"/>
       <c r="D10" s="17"/>
-      <c r="E10" s="25"/>
-      <c r="F10" s="17"/>
+      <c r="E10" s="22"/>
+      <c r="F10" s="22"/>
       <c r="G10" s="17"/>
-      <c r="H10" s="24"/>
+      <c r="H10" s="18"/>
       <c r="I10"/>
       <c r="J10"/>
       <c r="K10"/>
@@ -1414,11 +1410,11 @@
         <v>28</v>
       </c>
       <c r="B11" s="10"/>
-      <c r="C11" s="17"/>
+      <c r="C11" s="22"/>
       <c r="D11" s="17"/>
-      <c r="E11" s="22"/>
-      <c r="F11" s="22"/>
-      <c r="G11" s="17"/>
+      <c r="E11" s="17"/>
+      <c r="F11" s="17"/>
+      <c r="G11" s="22"/>
       <c r="H11" s="18"/>
       <c r="I11"/>
       <c r="J11"/>
@@ -1461,10 +1457,10 @@
         <v>29</v>
       </c>
       <c r="B12" s="10"/>
-      <c r="C12" s="22"/>
-      <c r="D12" s="17"/>
-      <c r="E12" s="17"/>
-      <c r="F12" s="17"/>
+      <c r="C12" s="17"/>
+      <c r="D12" s="25"/>
+      <c r="E12" s="22"/>
+      <c r="F12" s="22"/>
       <c r="G12" s="22"/>
       <c r="H12" s="18"/>
       <c r="I12"/>
@@ -1505,15 +1501,15 @@
     </row>
     <row r="13" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="11" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="B13" s="10"/>
-      <c r="C13" s="17"/>
-      <c r="D13" s="25"/>
-      <c r="E13" s="22"/>
-      <c r="F13" s="22"/>
-      <c r="G13" s="22"/>
-      <c r="H13" s="18"/>
+      <c r="C13" s="22"/>
+      <c r="D13" s="17"/>
+      <c r="E13" s="17"/>
+      <c r="F13" s="17"/>
+      <c r="G13" s="17"/>
+      <c r="H13" s="24"/>
       <c r="I13"/>
       <c r="J13"/>
       <c r="K13"/>
@@ -1552,15 +1548,15 @@
     </row>
     <row r="14" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="11" t="s">
-        <v>25</v>
+        <v>35</v>
       </c>
       <c r="B14" s="10"/>
-      <c r="C14" s="22"/>
-      <c r="D14" s="17"/>
-      <c r="E14" s="17"/>
-      <c r="F14" s="17"/>
-      <c r="G14" s="17"/>
-      <c r="H14" s="24"/>
+      <c r="C14" s="17"/>
+      <c r="D14" s="22"/>
+      <c r="E14" s="22"/>
+      <c r="F14" s="22"/>
+      <c r="G14" s="22"/>
+      <c r="H14" s="18"/>
       <c r="I14"/>
       <c r="J14"/>
       <c r="K14"/>
@@ -1599,15 +1595,15 @@
     </row>
     <row r="15" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="11" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B15" s="10"/>
-      <c r="C15" s="17"/>
-      <c r="D15" s="22"/>
-      <c r="E15" s="22"/>
+      <c r="C15" s="22"/>
+      <c r="D15" s="17"/>
+      <c r="E15" s="17"/>
       <c r="F15" s="22"/>
-      <c r="G15" s="22"/>
-      <c r="H15" s="18"/>
+      <c r="G15" s="17"/>
+      <c r="H15" s="24"/>
       <c r="I15"/>
       <c r="J15"/>
       <c r="K15"/>
@@ -1645,16 +1641,16 @@
       <c r="AQ15"/>
     </row>
     <row r="16" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="B16" s="10"/>
-      <c r="C16" s="22"/>
-      <c r="D16" s="17"/>
-      <c r="E16" s="17"/>
-      <c r="F16" s="22"/>
-      <c r="G16" s="17"/>
-      <c r="H16" s="24"/>
+      <c r="A16" s="40" t="s">
+        <v>20</v>
+      </c>
+      <c r="B16" s="41"/>
+      <c r="C16" s="41"/>
+      <c r="D16" s="41"/>
+      <c r="E16" s="41"/>
+      <c r="F16" s="41"/>
+      <c r="G16" s="41"/>
+      <c r="H16" s="42"/>
       <c r="I16"/>
       <c r="J16"/>
       <c r="K16"/>
@@ -1692,16 +1688,16 @@
       <c r="AQ16"/>
     </row>
     <row r="17" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="40" t="s">
-        <v>20</v>
-      </c>
-      <c r="B17" s="41"/>
-      <c r="C17" s="41"/>
-      <c r="D17" s="41"/>
-      <c r="E17" s="41"/>
-      <c r="F17" s="41"/>
-      <c r="G17" s="41"/>
-      <c r="H17" s="42"/>
+      <c r="A17" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="B17" s="10"/>
+      <c r="C17" s="22"/>
+      <c r="D17" s="22"/>
+      <c r="E17" s="17"/>
+      <c r="F17" s="22"/>
+      <c r="G17" s="22"/>
+      <c r="H17" s="24"/>
       <c r="I17"/>
       <c r="J17"/>
       <c r="K17"/>
@@ -1739,16 +1735,14 @@
       <c r="AQ17"/>
     </row>
     <row r="18" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="11" t="s">
-        <v>32</v>
-      </c>
+      <c r="A18" s="11"/>
       <c r="B18" s="10"/>
-      <c r="C18" s="22"/>
-      <c r="D18" s="22"/>
+      <c r="C18" s="17"/>
+      <c r="D18" s="17"/>
       <c r="E18" s="17"/>
-      <c r="F18" s="22"/>
-      <c r="G18" s="22"/>
-      <c r="H18" s="24"/>
+      <c r="F18" s="17"/>
+      <c r="G18" s="17"/>
+      <c r="H18" s="18"/>
       <c r="I18"/>
       <c r="J18"/>
       <c r="K18"/>
@@ -2011,14 +2005,16 @@
       <c r="AQ23"/>
     </row>
     <row r="24" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="11"/>
-      <c r="B24" s="10"/>
-      <c r="C24" s="17"/>
-      <c r="D24" s="17"/>
-      <c r="E24" s="17"/>
-      <c r="F24" s="17"/>
-      <c r="G24" s="17"/>
-      <c r="H24" s="18"/>
+      <c r="A24" s="40" t="s">
+        <v>21</v>
+      </c>
+      <c r="B24" s="41"/>
+      <c r="C24" s="41"/>
+      <c r="D24" s="41"/>
+      <c r="E24" s="41"/>
+      <c r="F24" s="41"/>
+      <c r="G24" s="41"/>
+      <c r="H24" s="42"/>
       <c r="I24"/>
       <c r="J24"/>
       <c r="K24"/>
@@ -2056,16 +2052,16 @@
       <c r="AQ24"/>
     </row>
     <row r="25" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="40" t="s">
-        <v>21</v>
-      </c>
-      <c r="B25" s="41"/>
-      <c r="C25" s="41"/>
-      <c r="D25" s="41"/>
-      <c r="E25" s="41"/>
-      <c r="F25" s="41"/>
-      <c r="G25" s="41"/>
-      <c r="H25" s="42"/>
+      <c r="A25" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="B25" s="10"/>
+      <c r="C25" s="22"/>
+      <c r="D25" s="22"/>
+      <c r="E25" s="17"/>
+      <c r="F25" s="22"/>
+      <c r="G25" s="22"/>
+      <c r="H25" s="24"/>
       <c r="I25"/>
       <c r="J25"/>
       <c r="K25"/>
@@ -2103,16 +2099,14 @@
       <c r="AQ25"/>
     </row>
     <row r="26" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="11" t="s">
-        <v>33</v>
-      </c>
+      <c r="A26" s="11"/>
       <c r="B26" s="10"/>
-      <c r="C26" s="22"/>
-      <c r="D26" s="22"/>
+      <c r="C26" s="17"/>
+      <c r="D26" s="17"/>
       <c r="E26" s="17"/>
-      <c r="F26" s="22"/>
-      <c r="G26" s="22"/>
-      <c r="H26" s="24"/>
+      <c r="F26" s="17"/>
+      <c r="G26" s="17"/>
+      <c r="H26" s="18"/>
       <c r="I26"/>
       <c r="J26"/>
       <c r="K26"/>
@@ -2329,15 +2323,15 @@
       <c r="AP30"/>
       <c r="AQ30"/>
     </row>
-    <row r="31" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="11"/>
-      <c r="B31" s="10"/>
-      <c r="C31" s="17"/>
-      <c r="D31" s="17"/>
-      <c r="E31" s="17"/>
-      <c r="F31" s="17"/>
-      <c r="G31" s="17"/>
-      <c r="H31" s="18"/>
+    <row r="31" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="12"/>
+      <c r="B31" s="13"/>
+      <c r="C31" s="19"/>
+      <c r="D31" s="19"/>
+      <c r="E31" s="19"/>
+      <c r="F31" s="19"/>
+      <c r="G31" s="19"/>
+      <c r="H31" s="20"/>
       <c r="I31"/>
       <c r="J31"/>
       <c r="K31"/>
@@ -2374,15 +2368,15 @@
       <c r="AP31"/>
       <c r="AQ31"/>
     </row>
-    <row r="32" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="12"/>
-      <c r="B32" s="13"/>
-      <c r="C32" s="19"/>
-      <c r="D32" s="19"/>
-      <c r="E32" s="19"/>
-      <c r="F32" s="19"/>
-      <c r="G32" s="19"/>
-      <c r="H32" s="20"/>
+    <row r="32" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="5"/>
+      <c r="B32" s="3"/>
+      <c r="C32" s="4"/>
+      <c r="D32" s="4"/>
+      <c r="E32" s="4"/>
+      <c r="F32" s="4"/>
+      <c r="G32" s="4"/>
+      <c r="H32" s="4"/>
       <c r="I32"/>
       <c r="J32"/>
       <c r="K32"/>
@@ -2420,14 +2414,14 @@
       <c r="AQ32"/>
     </row>
     <row r="33" spans="1:43" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="5"/>
-      <c r="B33" s="3"/>
-      <c r="C33" s="4"/>
-      <c r="D33" s="4"/>
-      <c r="E33" s="4"/>
-      <c r="F33" s="4"/>
-      <c r="G33" s="4"/>
-      <c r="H33" s="4"/>
+      <c r="A33"/>
+      <c r="B33"/>
+      <c r="C33"/>
+      <c r="D33"/>
+      <c r="E33"/>
+      <c r="F33"/>
+      <c r="G33"/>
+      <c r="H33"/>
       <c r="I33"/>
       <c r="J33"/>
       <c r="K33"/>
@@ -2685,7 +2679,16 @@
     <row r="76" spans="1:8" customFormat="1" x14ac:dyDescent="0.2"/>
     <row r="77" spans="1:8" customFormat="1" x14ac:dyDescent="0.2"/>
     <row r="78" spans="1:8" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="79" spans="1:8" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="79" spans="1:8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A79" s="1"/>
+      <c r="B79" s="1"/>
+      <c r="C79" s="1"/>
+      <c r="D79" s="1"/>
+      <c r="E79" s="1"/>
+      <c r="F79" s="1"/>
+      <c r="G79" s="1"/>
+      <c r="H79" s="1"/>
+    </row>
     <row r="80" spans="1:8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A80" s="1"/>
       <c r="B80" s="1"/>
@@ -2731,8 +2734,8 @@
     <mergeCell ref="A6:A7"/>
     <mergeCell ref="A2:H2"/>
     <mergeCell ref="A8:H8"/>
-    <mergeCell ref="A17:H17"/>
-    <mergeCell ref="A25:H25"/>
+    <mergeCell ref="A16:H16"/>
+    <mergeCell ref="A24:H24"/>
     <mergeCell ref="B6:B7"/>
     <mergeCell ref="A5:H5"/>
     <mergeCell ref="G1:H1"/>

</xml_diff>